<commit_message>
many updates for 1.0.18
</commit_message>
<xml_diff>
--- a/exampleFiles/TimeKex_timeData.xlsx
+++ b/exampleFiles/TimeKex_timeData.xlsx
@@ -1,38 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\git\reactdev\kimai-excel-import\public\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\git\TimeKex\exampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F446C1-5B6A-49E6-A0CB-E4608915F803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39A4617-B533-41E9-A05E-1ADF6335E547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1765BF24-13D1-4792-ADB5-4E37D4C61FFF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1765BF24-13D1-4792-ADB5-4E37D4C61FFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="TimeTracking" sheetId="2" r:id="rId1"/>
+    <sheet name="TimeTracking (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="TimeTracking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="25">
   <si>
     <t>Vacation</t>
   </si>
@@ -104,15 +98,19 @@
   </si>
   <si>
     <t>Line number</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -143,23 +141,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,11 +183,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2ED6F9ED-FDBF-4473-8C8B-CC345F51EC16}" name="Tabelle22" displayName="Tabelle22" ref="A1:J11" totalsRowShown="0">
+  <autoFilter ref="A1:J11" xr:uid="{AB7EBEAD-3C38-48E9-8E04-98DB0B096DED}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{B40C459F-F82E-4C6E-A9AA-7DE0B4BBABE6}" name="Line number"/>
+    <tableColumn id="6" xr3:uid="{C6598D34-B7BB-4507-9C76-E1DAEFFCD9E5}" name="Date" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{13B9F358-50E8-471B-B89F-540AFD7259EC}" name="Client"/>
+    <tableColumn id="4" xr3:uid="{8C4632DF-5CAA-45D4-B5BF-458EDFCB9AEB}" name="Project"/>
+    <tableColumn id="5" xr3:uid="{E72503E5-65FA-44A2-BE54-F8E29034BCFA}" name="Activity"/>
+    <tableColumn id="7" xr3:uid="{0A114683-4F48-4B42-AAE6-A7B109B84805}" name="chargeable"/>
+    <tableColumn id="9" xr3:uid="{A1A4997E-AAD6-40DB-8127-9C4423844E54}" name="Tasks"/>
+    <tableColumn id="10" xr3:uid="{81AC5AB7-5DFB-4C20-9163-E7AFF7BDCFCC}" name="Description"/>
+    <tableColumn id="11" xr3:uid="{6C7E2944-026B-47CB-9FD9-D2171294156D}" name="Start" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{0D54218B-13AA-4358-893B-29DA2A4D1A1D}" name="End" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB7EBEAD-3C38-48E9-8E04-98DB0B096DED}" name="Tabelle2" displayName="Tabelle2" ref="A1:K14" totalsRowShown="0">
   <autoFilter ref="A1:K14" xr:uid="{AB7EBEAD-3C38-48E9-8E04-98DB0B096DED}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{80E81A12-94FE-4ADE-A296-F156331A3356}" name="Line number"/>
-    <tableColumn id="2" xr3:uid="{8FA56BBC-C4DE-4FA7-9915-17B84CF612FB}" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8FA56BBC-C4DE-4FA7-9915-17B84CF612FB}" name="Date" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{BC5E3096-EEB4-4A22-A70B-2BB214292245}" name="Client"/>
     <tableColumn id="4" xr3:uid="{85F7CAAF-DDE7-428E-95C9-47D259BE6B06}" name="Project"/>
     <tableColumn id="5" xr3:uid="{7CD251AA-BDF1-4BA0-B538-D723643F3F86}" name="Activity"/>
@@ -187,8 +214,8 @@
     <tableColumn id="8" xr3:uid="{6785593A-0FB3-48F7-8A46-E2909C22F4CB}" name="chargeable (correction)"/>
     <tableColumn id="9" xr3:uid="{5DF9A9AC-7394-4D7A-BA46-AEADC94C50E1}" name="Tasks"/>
     <tableColumn id="10" xr3:uid="{F88DEFD3-9D44-4287-BFB4-13E199C677D0}" name="Details"/>
-    <tableColumn id="11" xr3:uid="{F63EE285-577D-4A8C-A6D6-065019780820}" name="Start" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{5D66738F-1988-4B79-827A-D5F63EB6DD3F}" name="End" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{F63EE285-577D-4A8C-A6D6-065019780820}" name="Start" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{5D66738F-1988-4B79-827A-D5F63EB6DD3F}" name="End" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,10 +517,379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDACD6C-347C-4BE4-ACA6-855226268989}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.65625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5612A3C0-D0E3-4BF4-AFC7-DE035A23A0FA}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates to support new API from ApprovalBundle 2.2 and up
</commit_message>
<xml_diff>
--- a/exampleFiles/TimeKex_timeData.xlsx
+++ b/exampleFiles/TimeKex_timeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\git\TimeKex\exampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\TimeKex\exampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28839B3E-72B4-4070-B990-6679C61A1847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9334C5C7-F48F-4204-B285-E4D8BF6329E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="1200" windowWidth="24705" windowHeight="11385" activeTab="1" xr2:uid="{1765BF24-13D1-4792-ADB5-4E37D4C61FFF}"/>
+    <workbookView xWindow="765" yWindow="1200" windowWidth="24705" windowHeight="11385" xr2:uid="{1765BF24-13D1-4792-ADB5-4E37D4C61FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTracking" sheetId="3" r:id="rId1"/>
@@ -109,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -225,7 +225,7 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -239,7 +239,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -252,7 +252,7 @@
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDACD6C-347C-4BE4-ACA6-855226268989}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -639,7 +639,7 @@
       </c>
       <c r="B2" s="2">
         <f>StartDayConfig!A2</f>
-        <v>45292</v>
+        <v>45658</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -669,7 +669,7 @@
       </c>
       <c r="B3" s="2">
         <f>StartDayConfig!A2+1</f>
-        <v>45293</v>
+        <v>45659</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="B4" s="2">
         <f>StartDayConfig!A2+2</f>
-        <v>45294</v>
+        <v>45660</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="B5" s="2">
         <f>StartDayConfig!A2+2</f>
-        <v>45294</v>
+        <v>45660</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -759,7 +759,7 @@
       </c>
       <c r="B6" s="2">
         <f>StartDayConfig!A2+3</f>
-        <v>45295</v>
+        <v>45661</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -792,7 +792,7 @@
       </c>
       <c r="B7" s="2">
         <f>StartDayConfig!A2+3</f>
-        <v>45295</v>
+        <v>45661</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="B8" s="2">
         <f>StartDayConfig!A2+3</f>
-        <v>45295</v>
+        <v>45661</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -858,7 +858,7 @@
       </c>
       <c r="B9" s="2">
         <f>StartDayConfig!A2+4</f>
-        <v>45296</v>
+        <v>45662</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="B10" s="2">
         <f>StartDayConfig!A2+4</f>
-        <v>45296</v>
+        <v>45662</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -924,7 +924,7 @@
       </c>
       <c r="B11" s="2">
         <f>StartDayConfig!A2+4</f>
-        <v>45296</v>
+        <v>45662</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -957,7 +957,7 @@
       </c>
       <c r="B12" s="2">
         <f>StartDayConfig!A2+7</f>
-        <v>45299</v>
+        <v>45665</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>1</v>
@@ -988,7 +988,7 @@
       </c>
       <c r="B13" s="2">
         <f>StartDayConfig!A2+8</f>
-        <v>45300</v>
+        <v>45666</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>1</v>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B14" s="2">
         <f>StartDayConfig!A2+9</f>
-        <v>45301</v>
+        <v>45667</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>1</v>
@@ -1057,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4F737A-48A3-41F4-94F0-FE5C9C387AA2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
-        <v>45292</v>
+        <v>45658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>